<commit_message>
Bug fixes and minor improvements
</commit_message>
<xml_diff>
--- a/workbooks/temp_rasp1.xlsx
+++ b/workbooks/temp_rasp1.xlsx
@@ -2548,6 +2548,33 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2557,35 +2584,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2956,20 +2956,20 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="37.799999999999997" x14ac:dyDescent="0.65">
-      <c r="G3" s="192" t="s">
+      <c r="G3" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="192"/>
-      <c r="M3" s="192"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="192"/>
-      <c r="P3" s="192"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="192"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="201"/>
+      <c r="J3" s="201"/>
+      <c r="K3" s="201"/>
+      <c r="L3" s="201"/>
+      <c r="M3" s="201"/>
+      <c r="N3" s="201"/>
+      <c r="O3" s="201"/>
+      <c r="P3" s="201"/>
+      <c r="Q3" s="201"/>
+      <c r="R3" s="201"/>
       <c r="T3" s="27" t="s">
         <v>5</v>
       </c>
@@ -2977,20 +2977,20 @@
     </row>
     <row r="4" spans="1:22" ht="35.4" x14ac:dyDescent="0.6">
       <c r="E4" s="3"/>
-      <c r="G4" s="193" t="s">
+      <c r="G4" s="202" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="193"/>
-      <c r="I4" s="193"/>
-      <c r="J4" s="193"/>
-      <c r="K4" s="193"/>
-      <c r="L4" s="193"/>
-      <c r="M4" s="193"/>
-      <c r="N4" s="193"/>
-      <c r="O4" s="193"/>
-      <c r="P4" s="193"/>
-      <c r="Q4" s="193"/>
-      <c r="R4" s="193"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="202"/>
       <c r="T4" s="25" t="s">
         <v>4</v>
       </c>
@@ -3000,14 +3000,14 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="193" t="s">
+      <c r="J5" s="202" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="193"/>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
-      <c r="N5" s="193"/>
-      <c r="O5" s="193"/>
+      <c r="K5" s="202"/>
+      <c r="L5" s="202"/>
+      <c r="M5" s="202"/>
+      <c r="N5" s="202"/>
+      <c r="O5" s="202"/>
       <c r="Q5" s="26"/>
       <c r="T5" s="26" t="s">
         <v>115</v>
@@ -3039,45 +3039,45 @@
       <c r="C7" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="203" t="s">
+      <c r="D7" s="199" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="204"/>
+      <c r="E7" s="200"/>
       <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="200" t="s">
+      <c r="G7" s="197" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="201"/>
+      <c r="H7" s="198"/>
       <c r="I7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="200" t="s">
+      <c r="J7" s="197" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="201"/>
+      <c r="K7" s="198"/>
       <c r="L7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="200" t="s">
+      <c r="M7" s="197" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="201"/>
+      <c r="N7" s="198"/>
       <c r="O7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="200" t="s">
+      <c r="P7" s="197" t="s">
         <v>48</v>
       </c>
-      <c r="Q7" s="201"/>
+      <c r="Q7" s="198"/>
       <c r="R7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="200" t="s">
+      <c r="S7" s="197" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="201"/>
+      <c r="T7" s="198"/>
       <c r="U7" s="35" t="s">
         <v>3</v>
       </c>
@@ -3086,7 +3086,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="195" t="s">
+      <c r="A8" s="192" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="177">
@@ -3113,12 +3113,12 @@
       <c r="U8" s="59">
         <v>1</v>
       </c>
-      <c r="V8" s="195" t="s">
+      <c r="V8" s="192" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="196"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="50">
         <v>2</v>
       </c>
@@ -3143,10 +3143,10 @@
       <c r="U9" s="52">
         <v>2</v>
       </c>
-      <c r="V9" s="196"/>
+      <c r="V9" s="193"/>
     </row>
     <row r="10" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="196"/>
+      <c r="A10" s="193"/>
       <c r="B10" s="50">
         <v>3</v>
       </c>
@@ -3171,10 +3171,10 @@
       <c r="U10" s="52">
         <v>3</v>
       </c>
-      <c r="V10" s="196"/>
+      <c r="V10" s="193"/>
     </row>
     <row r="11" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="197"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="178">
         <v>4</v>
       </c>
@@ -3199,10 +3199,10 @@
       <c r="U11" s="52">
         <v>4</v>
       </c>
-      <c r="V11" s="197"/>
+      <c r="V11" s="194"/>
     </row>
     <row r="12" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A12" s="197"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="178">
         <v>5</v>
       </c>
@@ -3227,10 +3227,10 @@
       <c r="U12" s="52">
         <v>5</v>
       </c>
-      <c r="V12" s="197"/>
+      <c r="V12" s="194"/>
     </row>
     <row r="13" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="197"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="179">
         <v>6</v>
       </c>
@@ -3255,10 +3255,10 @@
       <c r="U13" s="52">
         <v>6</v>
       </c>
-      <c r="V13" s="197"/>
+      <c r="V13" s="194"/>
     </row>
     <row r="14" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="192" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="61">
@@ -3309,12 +3309,12 @@
       <c r="U14" s="61">
         <v>1</v>
       </c>
-      <c r="V14" s="195" t="s">
+      <c r="V14" s="192" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="196"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="52">
         <v>2</v>
       </c>
@@ -3369,10 +3369,10 @@
       <c r="U15" s="52">
         <v>2</v>
       </c>
-      <c r="V15" s="196"/>
+      <c r="V15" s="193"/>
     </row>
     <row r="16" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="196"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="52">
         <v>3</v>
       </c>
@@ -3433,10 +3433,10 @@
       <c r="U16" s="52">
         <v>3</v>
       </c>
-      <c r="V16" s="196"/>
+      <c r="V16" s="193"/>
     </row>
     <row r="17" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="197"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="53">
         <v>4</v>
       </c>
@@ -3497,10 +3497,10 @@
       <c r="U17" s="52">
         <v>4</v>
       </c>
-      <c r="V17" s="197"/>
+      <c r="V17" s="194"/>
     </row>
     <row r="18" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="197"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="53">
         <v>5</v>
       </c>
@@ -3531,10 +3531,10 @@
       <c r="U18" s="52">
         <v>5</v>
       </c>
-      <c r="V18" s="197"/>
+      <c r="V18" s="194"/>
     </row>
     <row r="19" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="198"/>
+      <c r="A19" s="195"/>
       <c r="B19" s="60">
         <v>6</v>
       </c>
@@ -3559,10 +3559,10 @@
       <c r="U19" s="52">
         <v>6</v>
       </c>
-      <c r="V19" s="198"/>
+      <c r="V19" s="195"/>
     </row>
     <row r="20" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="202" t="s">
+      <c r="A20" s="196" t="s">
         <v>119</v>
       </c>
       <c r="B20" s="61">
@@ -3619,12 +3619,12 @@
       <c r="U20" s="61">
         <v>1</v>
       </c>
-      <c r="V20" s="202" t="s">
+      <c r="V20" s="196" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="196"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="52">
         <v>2</v>
       </c>
@@ -3685,10 +3685,10 @@
       <c r="U21" s="52">
         <v>2</v>
       </c>
-      <c r="V21" s="196"/>
+      <c r="V21" s="193"/>
     </row>
     <row r="22" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="196"/>
+      <c r="A22" s="193"/>
       <c r="B22" s="52">
         <v>3</v>
       </c>
@@ -3749,10 +3749,10 @@
       <c r="U22" s="52">
         <v>3</v>
       </c>
-      <c r="V22" s="196"/>
+      <c r="V22" s="193"/>
     </row>
     <row r="23" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="197"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="53">
         <v>4</v>
       </c>
@@ -3807,10 +3807,10 @@
       <c r="U23" s="53">
         <v>4</v>
       </c>
-      <c r="V23" s="197"/>
+      <c r="V23" s="194"/>
     </row>
     <row r="24" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="197"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="53">
         <v>5</v>
       </c>
@@ -3835,10 +3835,10 @@
       <c r="U24" s="53">
         <v>5</v>
       </c>
-      <c r="V24" s="197"/>
+      <c r="V24" s="194"/>
     </row>
     <row r="25" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="198"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="60">
         <v>6</v>
       </c>
@@ -3863,10 +3863,10 @@
       <c r="U25" s="60">
         <v>6</v>
       </c>
-      <c r="V25" s="198"/>
+      <c r="V25" s="195"/>
     </row>
     <row r="26" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="195" t="s">
+      <c r="A26" s="192" t="s">
         <v>120</v>
       </c>
       <c r="B26" s="61">
@@ -3929,12 +3929,12 @@
       <c r="U26" s="61">
         <v>1</v>
       </c>
-      <c r="V26" s="195" t="s">
+      <c r="V26" s="192" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="196"/>
+      <c r="A27" s="193"/>
       <c r="B27" s="62">
         <v>2</v>
       </c>
@@ -3995,10 +3995,10 @@
       <c r="U27" s="52">
         <v>2</v>
       </c>
-      <c r="V27" s="196"/>
+      <c r="V27" s="193"/>
     </row>
     <row r="28" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="196"/>
+      <c r="A28" s="193"/>
       <c r="B28" s="52">
         <v>3</v>
       </c>
@@ -4053,10 +4053,10 @@
       <c r="U28" s="52">
         <v>3</v>
       </c>
-      <c r="V28" s="196"/>
+      <c r="V28" s="193"/>
     </row>
     <row r="29" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="197"/>
+      <c r="A29" s="194"/>
       <c r="B29" s="53">
         <v>4</v>
       </c>
@@ -4099,10 +4099,10 @@
       <c r="U29" s="53">
         <v>4</v>
       </c>
-      <c r="V29" s="197"/>
+      <c r="V29" s="194"/>
     </row>
     <row r="30" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A30" s="197"/>
+      <c r="A30" s="194"/>
       <c r="B30" s="53">
         <v>5</v>
       </c>
@@ -4127,10 +4127,10 @@
       <c r="U30" s="53">
         <v>5</v>
       </c>
-      <c r="V30" s="197"/>
+      <c r="V30" s="194"/>
     </row>
     <row r="31" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="198"/>
+      <c r="A31" s="195"/>
       <c r="B31" s="60">
         <v>6</v>
       </c>
@@ -4155,10 +4155,10 @@
       <c r="U31" s="60">
         <v>6</v>
       </c>
-      <c r="V31" s="198"/>
+      <c r="V31" s="195"/>
     </row>
     <row r="32" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="195" t="s">
+      <c r="A32" s="192" t="s">
         <v>121</v>
       </c>
       <c r="B32" s="61">
@@ -4221,12 +4221,12 @@
       <c r="U32" s="61">
         <v>1</v>
       </c>
-      <c r="V32" s="195" t="s">
+      <c r="V32" s="192" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="196"/>
+      <c r="A33" s="193"/>
       <c r="B33" s="52">
         <v>2</v>
       </c>
@@ -4287,10 +4287,10 @@
       <c r="U33" s="52">
         <v>2</v>
       </c>
-      <c r="V33" s="196"/>
+      <c r="V33" s="193"/>
     </row>
     <row r="34" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="196"/>
+      <c r="A34" s="193"/>
       <c r="B34" s="52">
         <v>3</v>
       </c>
@@ -4345,10 +4345,10 @@
       <c r="U34" s="52">
         <v>3</v>
       </c>
-      <c r="V34" s="196"/>
+      <c r="V34" s="193"/>
     </row>
     <row r="35" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="196"/>
+      <c r="A35" s="193"/>
       <c r="B35" s="53">
         <v>4</v>
       </c>
@@ -4385,10 +4385,10 @@
       <c r="U35" s="53">
         <v>4</v>
       </c>
-      <c r="V35" s="196"/>
+      <c r="V35" s="193"/>
     </row>
     <row r="36" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="197"/>
+      <c r="A36" s="194"/>
       <c r="B36" s="53">
         <v>5</v>
       </c>
@@ -4413,10 +4413,10 @@
       <c r="U36" s="53">
         <v>5</v>
       </c>
-      <c r="V36" s="197"/>
+      <c r="V36" s="194"/>
     </row>
     <row r="37" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="198"/>
+      <c r="A37" s="195"/>
       <c r="B37" s="60">
         <v>6</v>
       </c>
@@ -4441,10 +4441,10 @@
       <c r="U37" s="60">
         <v>6</v>
       </c>
-      <c r="V37" s="198"/>
+      <c r="V37" s="195"/>
     </row>
     <row r="38" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="195" t="s">
+      <c r="A38" s="192" t="s">
         <v>122</v>
       </c>
       <c r="B38" s="62">
@@ -4495,12 +4495,12 @@
       <c r="U38" s="62">
         <v>1</v>
       </c>
-      <c r="V38" s="195" t="s">
+      <c r="V38" s="192" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="196"/>
+      <c r="A39" s="193"/>
       <c r="B39" s="52">
         <v>2</v>
       </c>
@@ -4561,10 +4561,10 @@
       <c r="U39" s="52">
         <v>2</v>
       </c>
-      <c r="V39" s="196"/>
+      <c r="V39" s="193"/>
     </row>
     <row r="40" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="196"/>
+      <c r="A40" s="193"/>
       <c r="B40" s="52">
         <v>3</v>
       </c>
@@ -4625,10 +4625,10 @@
       <c r="U40" s="52">
         <v>3</v>
       </c>
-      <c r="V40" s="196"/>
+      <c r="V40" s="193"/>
     </row>
     <row r="41" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="197"/>
+      <c r="A41" s="194"/>
       <c r="B41" s="57">
         <v>4</v>
       </c>
@@ -4677,10 +4677,10 @@
       <c r="U41" s="63">
         <v>4</v>
       </c>
-      <c r="V41" s="197"/>
+      <c r="V41" s="194"/>
     </row>
     <row r="42" spans="1:22" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A42" s="198"/>
+      <c r="A42" s="195"/>
       <c r="B42" s="60">
         <v>5</v>
       </c>
@@ -4705,67 +4705,60 @@
       <c r="U42" s="64">
         <v>5</v>
       </c>
-      <c r="V42" s="198"/>
+      <c r="V42" s="195"/>
     </row>
     <row r="43" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="199"/>
-      <c r="B43" s="199"/>
-      <c r="C43" s="199"/>
-      <c r="D43" s="199"/>
-      <c r="E43" s="199"/>
-      <c r="F43" s="199"/>
-      <c r="G43" s="199"/>
-      <c r="H43" s="199"/>
-      <c r="I43" s="199"/>
-      <c r="J43" s="199"/>
-      <c r="K43" s="199"/>
-      <c r="L43" s="199"/>
-      <c r="M43" s="199"/>
-      <c r="N43" s="199"/>
-      <c r="O43" s="199"/>
-      <c r="P43" s="199"/>
-      <c r="Q43" s="199"/>
-      <c r="R43" s="199"/>
-      <c r="S43" s="199"/>
-      <c r="T43" s="199"/>
-      <c r="U43" s="199"/>
-      <c r="V43" s="199"/>
+      <c r="A43" s="204"/>
+      <c r="B43" s="204"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="204"/>
+      <c r="E43" s="204"/>
+      <c r="F43" s="204"/>
+      <c r="G43" s="204"/>
+      <c r="H43" s="204"/>
+      <c r="I43" s="204"/>
+      <c r="J43" s="204"/>
+      <c r="K43" s="204"/>
+      <c r="L43" s="204"/>
+      <c r="M43" s="204"/>
+      <c r="N43" s="204"/>
+      <c r="O43" s="204"/>
+      <c r="P43" s="204"/>
+      <c r="Q43" s="204"/>
+      <c r="R43" s="204"/>
+      <c r="S43" s="204"/>
+      <c r="T43" s="204"/>
+      <c r="U43" s="204"/>
+      <c r="V43" s="204"/>
     </row>
     <row r="44" spans="1:22" ht="30" x14ac:dyDescent="0.4">
-      <c r="A44" s="194" t="s">
+      <c r="A44" s="203" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="194"/>
-      <c r="C44" s="194"/>
-      <c r="D44" s="194"/>
-      <c r="E44" s="194"/>
-      <c r="F44" s="194"/>
-      <c r="G44" s="194"/>
-      <c r="H44" s="194"/>
-      <c r="I44" s="194"/>
-      <c r="J44" s="194"/>
-      <c r="K44" s="194"/>
-      <c r="L44" s="194"/>
-      <c r="M44" s="194"/>
-      <c r="N44" s="194"/>
-      <c r="O44" s="194"/>
-      <c r="P44" s="194"/>
-      <c r="Q44" s="194"/>
-      <c r="R44" s="194"/>
-      <c r="S44" s="194"/>
-      <c r="T44" s="194"/>
-      <c r="U44" s="194"/>
-      <c r="V44" s="194"/>
+      <c r="B44" s="203"/>
+      <c r="C44" s="203"/>
+      <c r="D44" s="203"/>
+      <c r="E44" s="203"/>
+      <c r="F44" s="203"/>
+      <c r="G44" s="203"/>
+      <c r="H44" s="203"/>
+      <c r="I44" s="203"/>
+      <c r="J44" s="203"/>
+      <c r="K44" s="203"/>
+      <c r="L44" s="203"/>
+      <c r="M44" s="203"/>
+      <c r="N44" s="203"/>
+      <c r="O44" s="203"/>
+      <c r="P44" s="203"/>
+      <c r="Q44" s="203"/>
+      <c r="R44" s="203"/>
+      <c r="S44" s="203"/>
+      <c r="T44" s="203"/>
+      <c r="U44" s="203"/>
+      <c r="V44" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="V20:V25"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="G3:R3"/>
     <mergeCell ref="G4:R4"/>
     <mergeCell ref="A44:V44"/>
@@ -4782,6 +4775,13 @@
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="J5:O5"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="V20:V25"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.35433070866141736" right="0" top="0.59055118110236227" bottom="0" header="0" footer="0"/>
@@ -4797,8 +4797,8 @@
   </sheetPr>
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="L1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6:V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.6" x14ac:dyDescent="0.4"/>
@@ -4836,16 +4836,16 @@
       <c r="U1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="37.799999999999997" x14ac:dyDescent="0.65">
-      <c r="G2" s="192" t="s">
+      <c r="G2" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="201"/>
+      <c r="L2" s="201"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="201"/>
       <c r="O2" s="10"/>
       <c r="T2" s="27" t="s">
         <v>5</v>
@@ -4859,16 +4859,16 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="193" t="s">
+      <c r="G3" s="202" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="193"/>
-      <c r="L3" s="193"/>
-      <c r="M3" s="193"/>
-      <c r="N3" s="193"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
       <c r="O3" s="7"/>
       <c r="S3" s="2"/>
       <c r="T3" s="25" t="s">
@@ -4886,10 +4886,10 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="193" t="s">
+      <c r="J4" s="202" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="193"/>
+      <c r="K4" s="202"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="2"/>
@@ -4965,7 +4965,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="195" t="s">
+      <c r="A7" s="192" t="s">
         <v>118</v>
       </c>
       <c r="B7" s="55">
@@ -4992,12 +4992,12 @@
       <c r="U7" s="55">
         <v>1</v>
       </c>
-      <c r="V7" s="195" t="s">
+      <c r="V7" s="192" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="196"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="45">
         <v>2</v>
       </c>
@@ -5022,10 +5022,10 @@
       <c r="U8" s="45">
         <v>2</v>
       </c>
-      <c r="V8" s="196"/>
+      <c r="V8" s="193"/>
     </row>
     <row r="9" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="196"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="45">
         <v>3</v>
       </c>
@@ -5050,10 +5050,10 @@
       <c r="U9" s="45">
         <v>3</v>
       </c>
-      <c r="V9" s="196"/>
+      <c r="V9" s="193"/>
     </row>
     <row r="10" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="197"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="46">
         <v>4</v>
       </c>
@@ -5078,10 +5078,10 @@
       <c r="U10" s="46">
         <v>4</v>
       </c>
-      <c r="V10" s="197"/>
+      <c r="V10" s="194"/>
     </row>
     <row r="11" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="197"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="45">
         <v>5</v>
       </c>
@@ -5106,10 +5106,10 @@
       <c r="U11" s="46">
         <v>5</v>
       </c>
-      <c r="V11" s="197"/>
+      <c r="V11" s="194"/>
     </row>
     <row r="12" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A12" s="197"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="46">
         <v>6</v>
       </c>
@@ -5134,10 +5134,10 @@
       <c r="U12" s="47">
         <v>6</v>
       </c>
-      <c r="V12" s="197"/>
+      <c r="V12" s="194"/>
     </row>
     <row r="13" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="192" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="44">
@@ -5188,12 +5188,12 @@
       <c r="U13" s="44">
         <v>1</v>
       </c>
-      <c r="V13" s="195" t="s">
+      <c r="V13" s="192" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="196"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="45">
         <v>2</v>
       </c>
@@ -5254,10 +5254,10 @@
       <c r="U14" s="45">
         <v>2</v>
       </c>
-      <c r="V14" s="196"/>
+      <c r="V14" s="193"/>
     </row>
     <row r="15" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="196"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="45">
         <v>3</v>
       </c>
@@ -5318,10 +5318,10 @@
       <c r="U15" s="45">
         <v>3</v>
       </c>
-      <c r="V15" s="196"/>
+      <c r="V15" s="193"/>
     </row>
     <row r="16" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="197"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="46">
         <v>4</v>
       </c>
@@ -5370,10 +5370,10 @@
       <c r="U16" s="46">
         <v>4</v>
       </c>
-      <c r="V16" s="197"/>
+      <c r="V16" s="194"/>
     </row>
     <row r="17" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="197"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="45">
         <v>5</v>
       </c>
@@ -5404,10 +5404,10 @@
       <c r="U17" s="46">
         <v>5</v>
       </c>
-      <c r="V17" s="197"/>
+      <c r="V17" s="194"/>
     </row>
     <row r="18" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="198"/>
+      <c r="A18" s="195"/>
       <c r="B18" s="46">
         <v>6</v>
       </c>
@@ -5432,10 +5432,10 @@
       <c r="U18" s="47">
         <v>6</v>
       </c>
-      <c r="V18" s="198"/>
+      <c r="V18" s="195"/>
     </row>
     <row r="19" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="202" t="s">
+      <c r="A19" s="196" t="s">
         <v>119</v>
       </c>
       <c r="B19" s="44">
@@ -5486,12 +5486,12 @@
       <c r="U19" s="44">
         <v>1</v>
       </c>
-      <c r="V19" s="202" t="s">
+      <c r="V19" s="196" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="196"/>
+      <c r="A20" s="193"/>
       <c r="B20" s="45">
         <v>2</v>
       </c>
@@ -5540,10 +5540,10 @@
       <c r="U20" s="45">
         <v>2</v>
       </c>
-      <c r="V20" s="196"/>
+      <c r="V20" s="193"/>
     </row>
     <row r="21" spans="1:22" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A21" s="196"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="45">
         <v>3</v>
       </c>
@@ -5604,10 +5604,10 @@
       <c r="U21" s="45">
         <v>3</v>
       </c>
-      <c r="V21" s="196"/>
+      <c r="V21" s="193"/>
     </row>
     <row r="22" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="197"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="46">
         <v>4</v>
       </c>
@@ -5662,10 +5662,10 @@
       <c r="U22" s="46">
         <v>4</v>
       </c>
-      <c r="V22" s="197"/>
+      <c r="V22" s="194"/>
     </row>
     <row r="23" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="197"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="46">
         <v>5</v>
       </c>
@@ -5702,10 +5702,10 @@
       <c r="U23" s="46">
         <v>5</v>
       </c>
-      <c r="V23" s="197"/>
+      <c r="V23" s="194"/>
     </row>
     <row r="24" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="198"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="47">
         <v>6</v>
       </c>
@@ -5730,10 +5730,10 @@
       <c r="U24" s="47">
         <v>6</v>
       </c>
-      <c r="V24" s="198"/>
+      <c r="V24" s="195"/>
     </row>
     <row r="25" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="192" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="44">
@@ -5790,12 +5790,12 @@
       <c r="U25" s="44">
         <v>1</v>
       </c>
-      <c r="V25" s="195" t="s">
+      <c r="V25" s="192" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="196"/>
+      <c r="A26" s="193"/>
       <c r="B26" s="56">
         <v>2</v>
       </c>
@@ -5856,10 +5856,10 @@
       <c r="U26" s="45">
         <v>2</v>
       </c>
-      <c r="V26" s="196"/>
+      <c r="V26" s="193"/>
     </row>
     <row r="27" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="196"/>
+      <c r="A27" s="193"/>
       <c r="B27" s="45">
         <v>3</v>
       </c>
@@ -5914,10 +5914,10 @@
       <c r="U27" s="45">
         <v>3</v>
       </c>
-      <c r="V27" s="196"/>
+      <c r="V27" s="193"/>
     </row>
     <row r="28" spans="1:22" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A28" s="197"/>
+      <c r="A28" s="194"/>
       <c r="B28" s="46">
         <v>4</v>
       </c>
@@ -5972,10 +5972,10 @@
       <c r="U28" s="46">
         <v>4</v>
       </c>
-      <c r="V28" s="197"/>
+      <c r="V28" s="194"/>
     </row>
     <row r="29" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="197"/>
+      <c r="A29" s="194"/>
       <c r="B29" s="46">
         <v>5</v>
       </c>
@@ -6000,10 +6000,10 @@
       <c r="U29" s="46">
         <v>5</v>
       </c>
-      <c r="V29" s="197"/>
+      <c r="V29" s="194"/>
     </row>
     <row r="30" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="198"/>
+      <c r="A30" s="195"/>
       <c r="B30" s="47">
         <v>6</v>
       </c>
@@ -6028,10 +6028,10 @@
       <c r="U30" s="47">
         <v>6</v>
       </c>
-      <c r="V30" s="198"/>
+      <c r="V30" s="195"/>
     </row>
     <row r="31" spans="1:22" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="195" t="s">
+      <c r="A31" s="192" t="s">
         <v>121</v>
       </c>
       <c r="B31" s="44">
@@ -6070,12 +6070,12 @@
       <c r="U31" s="44">
         <v>1</v>
       </c>
-      <c r="V31" s="195" t="s">
+      <c r="V31" s="192" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="196"/>
+      <c r="A32" s="193"/>
       <c r="B32" s="45">
         <v>2</v>
       </c>
@@ -6130,10 +6130,10 @@
       <c r="U32" s="45">
         <v>2</v>
       </c>
-      <c r="V32" s="196"/>
+      <c r="V32" s="193"/>
     </row>
     <row r="33" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="196"/>
+      <c r="A33" s="193"/>
       <c r="B33" s="45">
         <v>3</v>
       </c>
@@ -6194,10 +6194,10 @@
       <c r="U33" s="45">
         <v>3</v>
       </c>
-      <c r="V33" s="196"/>
+      <c r="V33" s="193"/>
     </row>
     <row r="34" spans="1:22" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A34" s="196"/>
+      <c r="A34" s="193"/>
       <c r="B34" s="46">
         <v>4</v>
       </c>
@@ -6252,10 +6252,10 @@
       <c r="U34" s="46">
         <v>4</v>
       </c>
-      <c r="V34" s="196"/>
+      <c r="V34" s="193"/>
     </row>
     <row r="35" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="197"/>
+      <c r="A35" s="194"/>
       <c r="B35" s="46">
         <v>5</v>
       </c>
@@ -6298,10 +6298,10 @@
       <c r="U35" s="46">
         <v>5</v>
       </c>
-      <c r="V35" s="197"/>
+      <c r="V35" s="194"/>
     </row>
     <row r="36" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="198"/>
+      <c r="A36" s="195"/>
       <c r="B36" s="47">
         <v>6</v>
       </c>
@@ -6326,10 +6326,10 @@
       <c r="U36" s="47">
         <v>6</v>
       </c>
-      <c r="V36" s="198"/>
+      <c r="V36" s="195"/>
     </row>
     <row r="37" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="195" t="s">
+      <c r="A37" s="192" t="s">
         <v>122</v>
       </c>
       <c r="B37" s="56">
@@ -6386,12 +6386,12 @@
       <c r="U37" s="56">
         <v>1</v>
       </c>
-      <c r="V37" s="195" t="s">
+      <c r="V37" s="192" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A38" s="196"/>
+      <c r="A38" s="193"/>
       <c r="B38" s="45">
         <v>2</v>
       </c>
@@ -6446,10 +6446,10 @@
       <c r="U38" s="45">
         <v>2</v>
       </c>
-      <c r="V38" s="196"/>
+      <c r="V38" s="193"/>
     </row>
     <row r="39" spans="1:22" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A39" s="196"/>
+      <c r="A39" s="193"/>
       <c r="B39" s="45">
         <v>3</v>
       </c>
@@ -6510,10 +6510,10 @@
       <c r="U39" s="45">
         <v>3</v>
       </c>
-      <c r="V39" s="196"/>
+      <c r="V39" s="193"/>
     </row>
     <row r="40" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="197"/>
+      <c r="A40" s="194"/>
       <c r="B40" s="57">
         <v>4</v>
       </c>
@@ -6556,10 +6556,10 @@
       <c r="U40" s="57">
         <v>4</v>
       </c>
-      <c r="V40" s="197"/>
+      <c r="V40" s="194"/>
     </row>
     <row r="41" spans="1:22" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A41" s="198"/>
+      <c r="A41" s="195"/>
       <c r="B41" s="47">
         <v>5</v>
       </c>
@@ -6584,7 +6584,7 @@
       <c r="U41" s="47">
         <v>5</v>
       </c>
-      <c r="V41" s="198"/>
+      <c r="V41" s="195"/>
     </row>
     <row r="42" spans="1:22" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A42" s="207"/>
@@ -6637,6 +6637,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G3:N3"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="A42:S42"/>
     <mergeCell ref="A43:S43"/>
@@ -6653,13 +6660,6 @@
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="V19:V24"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G3:N3"/>
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="11" orientation="landscape" r:id="rId1"/>
@@ -6674,7 +6674,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" zoomScaleSheetLayoutView="54" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="A7" sqref="A7:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.6" x14ac:dyDescent="0.4"/>
@@ -6726,16 +6726,16 @@
       <c r="D2" s="13"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="192" t="s">
+      <c r="G2" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="201"/>
+      <c r="L2" s="201"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="201"/>
       <c r="Q2" s="168" t="s">
         <v>5</v>
       </c>
@@ -6747,16 +6747,16 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="193" t="s">
+      <c r="G3" s="202" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="193"/>
-      <c r="L3" s="193"/>
-      <c r="M3" s="193"/>
-      <c r="N3" s="193"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
       <c r="Q3" s="169" t="s">
         <v>4</v>
       </c>
@@ -6770,10 +6770,10 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="193" t="s">
+      <c r="J4" s="202" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="193"/>
+      <c r="K4" s="202"/>
       <c r="L4" s="19"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -6799,31 +6799,31 @@
       <c r="F6" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="200" t="s">
+      <c r="G6" s="197" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="201"/>
+      <c r="H6" s="198"/>
       <c r="I6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="200" t="s">
+      <c r="J6" s="197" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="201"/>
+      <c r="K6" s="198"/>
       <c r="L6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="200" t="s">
+      <c r="M6" s="197" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="201"/>
+      <c r="N6" s="198"/>
       <c r="O6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="200" t="s">
+      <c r="P6" s="197" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="201"/>
+      <c r="Q6" s="198"/>
       <c r="R6" s="51" t="s">
         <v>3</v>
       </c>
@@ -6832,7 +6832,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="195" t="s">
+      <c r="A7" s="192" t="s">
         <v>118</v>
       </c>
       <c r="B7" s="41">
@@ -6856,12 +6856,12 @@
       <c r="R7" s="44">
         <v>1</v>
       </c>
-      <c r="S7" s="195" t="s">
+      <c r="S7" s="192" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="196"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="42">
         <v>2</v>
       </c>
@@ -6883,10 +6883,10 @@
       <c r="R8" s="45">
         <v>2</v>
       </c>
-      <c r="S8" s="196"/>
+      <c r="S8" s="193"/>
     </row>
     <row r="9" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="196"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="42">
         <v>3</v>
       </c>
@@ -6908,10 +6908,10 @@
       <c r="R9" s="45">
         <v>3</v>
       </c>
-      <c r="S9" s="196"/>
+      <c r="S9" s="193"/>
     </row>
     <row r="10" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="197"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="43">
         <v>4</v>
       </c>
@@ -6933,10 +6933,10 @@
       <c r="R10" s="46">
         <v>4</v>
       </c>
-      <c r="S10" s="197"/>
+      <c r="S10" s="194"/>
     </row>
     <row r="11" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="197"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="43">
         <v>5</v>
       </c>
@@ -6958,10 +6958,10 @@
       <c r="R11" s="46">
         <v>5</v>
       </c>
-      <c r="S11" s="197"/>
+      <c r="S11" s="194"/>
     </row>
     <row r="12" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="197"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="43">
         <v>6</v>
       </c>
@@ -6983,10 +6983,10 @@
       <c r="R12" s="47">
         <v>6</v>
       </c>
-      <c r="S12" s="197"/>
+      <c r="S12" s="194"/>
     </row>
     <row r="13" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="192" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="44">
@@ -7034,12 +7034,12 @@
       <c r="R13" s="41">
         <v>1</v>
       </c>
-      <c r="S13" s="195" t="s">
+      <c r="S13" s="192" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="74.400000000000006" x14ac:dyDescent="0.4">
-      <c r="A14" s="196"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="45">
         <v>2</v>
       </c>
@@ -7085,10 +7085,10 @@
       <c r="R14" s="42">
         <v>2</v>
       </c>
-      <c r="S14" s="196"/>
+      <c r="S14" s="193"/>
     </row>
     <row r="15" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="196"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="45">
         <v>3</v>
       </c>
@@ -7140,10 +7140,10 @@
       <c r="R15" s="42">
         <v>3</v>
       </c>
-      <c r="S15" s="196"/>
+      <c r="S15" s="193"/>
     </row>
     <row r="16" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="197"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="46">
         <v>4</v>
       </c>
@@ -7189,10 +7189,10 @@
       <c r="R16" s="43">
         <v>4</v>
       </c>
-      <c r="S16" s="197"/>
+      <c r="S16" s="194"/>
     </row>
     <row r="17" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="197"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="45">
         <v>5</v>
       </c>
@@ -7220,10 +7220,10 @@
       <c r="R17" s="42">
         <v>5</v>
       </c>
-      <c r="S17" s="197"/>
+      <c r="S17" s="194"/>
     </row>
     <row r="18" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="198"/>
+      <c r="A18" s="195"/>
       <c r="B18" s="47">
         <v>6</v>
       </c>
@@ -7245,10 +7245,10 @@
       <c r="R18" s="49">
         <v>6</v>
       </c>
-      <c r="S18" s="198"/>
+      <c r="S18" s="195"/>
     </row>
     <row r="19" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="202" t="s">
+      <c r="A19" s="196" t="s">
         <v>119</v>
       </c>
       <c r="B19" s="48">
@@ -7296,12 +7296,12 @@
       <c r="R19" s="44">
         <v>1</v>
       </c>
-      <c r="S19" s="202" t="s">
+      <c r="S19" s="196" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="196"/>
+      <c r="A20" s="193"/>
       <c r="B20" s="42">
         <v>2</v>
       </c>
@@ -7353,10 +7353,10 @@
       <c r="R20" s="45">
         <v>2</v>
       </c>
-      <c r="S20" s="196"/>
+      <c r="S20" s="193"/>
     </row>
     <row r="21" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="196"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="42">
         <v>3</v>
       </c>
@@ -7408,10 +7408,10 @@
       <c r="R21" s="45">
         <v>3</v>
       </c>
-      <c r="S21" s="196"/>
+      <c r="S21" s="193"/>
     </row>
     <row r="22" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="197"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="43">
         <v>4</v>
       </c>
@@ -7451,10 +7451,10 @@
       <c r="R22" s="46">
         <v>4</v>
       </c>
-      <c r="S22" s="197"/>
+      <c r="S22" s="194"/>
     </row>
     <row r="23" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="197"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="42">
         <v>5</v>
       </c>
@@ -7476,10 +7476,10 @@
       <c r="R23" s="46">
         <v>5</v>
       </c>
-      <c r="S23" s="197"/>
+      <c r="S23" s="194"/>
     </row>
     <row r="24" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="198"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="49">
         <v>6</v>
       </c>
@@ -7501,10 +7501,10 @@
       <c r="R24" s="47">
         <v>6</v>
       </c>
-      <c r="S24" s="198"/>
+      <c r="S24" s="195"/>
     </row>
     <row r="25" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="192" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="41">
@@ -7552,12 +7552,12 @@
       <c r="R25" s="41">
         <v>1</v>
       </c>
-      <c r="S25" s="195" t="s">
+      <c r="S25" s="192" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="196"/>
+      <c r="A26" s="193"/>
       <c r="B26" s="42">
         <v>2</v>
       </c>
@@ -7609,10 +7609,10 @@
       <c r="R26" s="42">
         <v>2</v>
       </c>
-      <c r="S26" s="196"/>
+      <c r="S26" s="193"/>
     </row>
     <row r="27" spans="1:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="196"/>
+      <c r="A27" s="193"/>
       <c r="B27" s="42">
         <v>3</v>
       </c>
@@ -7664,10 +7664,10 @@
       <c r="R27" s="42">
         <v>3</v>
       </c>
-      <c r="S27" s="196"/>
+      <c r="S27" s="193"/>
     </row>
     <row r="28" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="197"/>
+      <c r="A28" s="194"/>
       <c r="B28" s="43">
         <v>4</v>
       </c>
@@ -7719,10 +7719,10 @@
       <c r="R28" s="43">
         <v>4</v>
       </c>
-      <c r="S28" s="197"/>
+      <c r="S28" s="194"/>
     </row>
     <row r="29" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="197"/>
+      <c r="A29" s="194"/>
       <c r="B29" s="42">
         <v>5</v>
       </c>
@@ -7750,10 +7750,10 @@
       <c r="R29" s="43">
         <v>5</v>
       </c>
-      <c r="S29" s="197"/>
+      <c r="S29" s="194"/>
     </row>
     <row r="30" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="198"/>
+      <c r="A30" s="195"/>
       <c r="B30" s="49">
         <v>6</v>
       </c>
@@ -7775,10 +7775,10 @@
       <c r="R30" s="49">
         <v>6</v>
       </c>
-      <c r="S30" s="198"/>
+      <c r="S30" s="195"/>
     </row>
     <row r="31" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="195" t="s">
+      <c r="A31" s="192" t="s">
         <v>121</v>
       </c>
       <c r="B31" s="44">
@@ -7826,12 +7826,12 @@
       <c r="R31" s="41">
         <v>1</v>
       </c>
-      <c r="S31" s="195" t="s">
+      <c r="S31" s="192" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="196"/>
+      <c r="A32" s="193"/>
       <c r="B32" s="45">
         <v>2</v>
       </c>
@@ -7883,10 +7883,10 @@
       <c r="R32" s="42">
         <v>2</v>
       </c>
-      <c r="S32" s="196"/>
+      <c r="S32" s="193"/>
     </row>
     <row r="33" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="196"/>
+      <c r="A33" s="193"/>
       <c r="B33" s="45">
         <v>3</v>
       </c>
@@ -7932,10 +7932,10 @@
       <c r="R33" s="42">
         <v>3</v>
       </c>
-      <c r="S33" s="196"/>
+      <c r="S33" s="193"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="196"/>
+      <c r="A34" s="193"/>
       <c r="B34" s="46">
         <v>4</v>
       </c>
@@ -7969,10 +7969,10 @@
       <c r="R34" s="43">
         <v>4</v>
       </c>
-      <c r="S34" s="196"/>
+      <c r="S34" s="193"/>
     </row>
     <row r="35" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="197"/>
+      <c r="A35" s="194"/>
       <c r="B35" s="45">
         <v>5</v>
       </c>
@@ -8000,10 +8000,10 @@
       <c r="R35" s="43">
         <v>5</v>
       </c>
-      <c r="S35" s="197"/>
+      <c r="S35" s="194"/>
     </row>
     <row r="36" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="198"/>
+      <c r="A36" s="195"/>
       <c r="B36" s="47">
         <v>6</v>
       </c>
@@ -8025,10 +8025,10 @@
       <c r="R36" s="49">
         <v>6</v>
       </c>
-      <c r="S36" s="198"/>
+      <c r="S36" s="195"/>
     </row>
     <row r="37" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="195" t="s">
+      <c r="A37" s="192" t="s">
         <v>122</v>
       </c>
       <c r="B37" s="41">
@@ -8076,12 +8076,12 @@
       <c r="R37" s="44">
         <v>1</v>
       </c>
-      <c r="S37" s="195" t="s">
+      <c r="S37" s="192" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="196"/>
+      <c r="A38" s="193"/>
       <c r="B38" s="42">
         <v>2</v>
       </c>
@@ -8133,10 +8133,10 @@
       <c r="R38" s="45">
         <v>2</v>
       </c>
-      <c r="S38" s="196"/>
+      <c r="S38" s="193"/>
     </row>
     <row r="39" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="196"/>
+      <c r="A39" s="193"/>
       <c r="B39" s="50">
         <v>3</v>
       </c>
@@ -8182,10 +8182,10 @@
       <c r="R39" s="52">
         <v>3</v>
       </c>
-      <c r="S39" s="196"/>
+      <c r="S39" s="193"/>
     </row>
     <row r="40" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="197"/>
+      <c r="A40" s="194"/>
       <c r="B40" s="42">
         <v>4</v>
       </c>
@@ -8225,10 +8225,10 @@
       <c r="R40" s="53">
         <v>4</v>
       </c>
-      <c r="S40" s="197"/>
+      <c r="S40" s="194"/>
     </row>
     <row r="41" spans="1:19" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="198"/>
+      <c r="A41" s="195"/>
       <c r="B41" s="49">
         <v>5</v>
       </c>
@@ -8250,7 +8250,7 @@
       <c r="R41" s="47">
         <v>5</v>
       </c>
-      <c r="S41" s="198"/>
+      <c r="S41" s="195"/>
     </row>
     <row r="42" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="21"/>
@@ -8292,6 +8292,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="G2:N2"/>
     <mergeCell ref="G3:N3"/>
     <mergeCell ref="D6:E6"/>
@@ -8308,11 +8313,6 @@
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.74803149606299213" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>